<commit_message>
update case ut FromHistory
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/TodayOdrRepository/FromHistorySample.xlsx
+++ b/CloudTest/SampleData/TodayOdrRepository/FromHistorySample.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SmartKarteBE\emr-cloud-be\CloudTest\SampleData\TodayOdrRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D30276-05C5-43DE-9755-047AE2BD45AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E9429B-A658-4CB1-8AF0-8F96D2080DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TenMst" sheetId="1" r:id="rId1"/>
-    <sheet name="YohoSetMst" sheetId="4" r:id="rId2"/>
-    <sheet name="IpnKasanExclude" sheetId="5" r:id="rId3"/>
-    <sheet name="IpnKasanExcludeItem" sheetId="6" r:id="rId4"/>
-    <sheet name="KensaMst" sheetId="2" r:id="rId5"/>
-    <sheet name="IpnNameMst" sheetId="3" r:id="rId6"/>
+    <sheet name="SystemConf" sheetId="7" state="hidden" r:id="rId2"/>
+    <sheet name="YohoSetMst" sheetId="4" r:id="rId3"/>
+    <sheet name="IpnKasanExclude" sheetId="5" r:id="rId4"/>
+    <sheet name="IpnKasanExcludeItem" sheetId="6" r:id="rId5"/>
+    <sheet name="KensaMst" sheetId="2" r:id="rId6"/>
+    <sheet name="IpnNameMst" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="252">
   <si>
     <t>HP_ID</t>
   </si>
@@ -768,6 +769,24 @@
   </si>
   <si>
     <t>item_cd</t>
+  </si>
+  <si>
+    <t>grp_cd</t>
+  </si>
+  <si>
+    <t>grp_eda_no</t>
+  </si>
+  <si>
+    <t>val</t>
+  </si>
+  <si>
+    <t>param</t>
+  </si>
+  <si>
+    <t>biko</t>
+  </si>
+  <si>
+    <t>ItemCd3</t>
   </si>
 </sst>
 </file>
@@ -1086,10 +1105,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:GG4"/>
+  <dimension ref="A1:GG5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="DE11" sqref="DE11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3109,17 +3128,578 @@
         <v>0</v>
       </c>
     </row>
+    <row r="5" spans="1:189" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>251</v>
+      </c>
+      <c r="C5">
+        <v>20220403</v>
+      </c>
+      <c r="D5">
+        <v>20250331</v>
+      </c>
+      <c r="E5" t="s">
+        <v>190</v>
+      </c>
+      <c r="F5">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
+        <v>191</v>
+      </c>
+      <c r="H5" t="s">
+        <v>192</v>
+      </c>
+      <c r="I5" t="s">
+        <v>193</v>
+      </c>
+      <c r="P5" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>12</v>
+      </c>
+      <c r="S5">
+        <v>33</v>
+      </c>
+      <c r="T5" t="s">
+        <v>195</v>
+      </c>
+      <c r="U5" t="s">
+        <v>195</v>
+      </c>
+      <c r="W5" t="s">
+        <v>196</v>
+      </c>
+      <c r="X5" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>197</v>
+      </c>
+      <c r="Z5">
+        <v>1</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <v>0</v>
+      </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5">
+        <v>0</v>
+      </c>
+      <c r="AK5">
+        <v>0</v>
+      </c>
+      <c r="AL5">
+        <v>0</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>196</v>
+      </c>
+      <c r="AN5">
+        <v>0</v>
+      </c>
+      <c r="AO5">
+        <v>0</v>
+      </c>
+      <c r="AP5">
+        <v>0</v>
+      </c>
+      <c r="AQ5">
+        <v>0</v>
+      </c>
+      <c r="AR5">
+        <v>0</v>
+      </c>
+      <c r="AS5">
+        <v>0</v>
+      </c>
+      <c r="AV5">
+        <v>0</v>
+      </c>
+      <c r="AW5">
+        <v>0</v>
+      </c>
+      <c r="AX5">
+        <v>0</v>
+      </c>
+      <c r="AY5">
+        <v>0</v>
+      </c>
+      <c r="AZ5">
+        <v>0</v>
+      </c>
+      <c r="BA5">
+        <v>0</v>
+      </c>
+      <c r="BB5">
+        <v>0</v>
+      </c>
+      <c r="BC5">
+        <v>0</v>
+      </c>
+      <c r="BD5">
+        <v>0</v>
+      </c>
+      <c r="BE5">
+        <v>0</v>
+      </c>
+      <c r="BF5">
+        <v>0</v>
+      </c>
+      <c r="BG5">
+        <v>0</v>
+      </c>
+      <c r="BH5">
+        <v>0</v>
+      </c>
+      <c r="BI5">
+        <v>0</v>
+      </c>
+      <c r="BJ5">
+        <v>0</v>
+      </c>
+      <c r="BK5">
+        <v>0</v>
+      </c>
+      <c r="BL5">
+        <v>0</v>
+      </c>
+      <c r="BM5">
+        <v>0</v>
+      </c>
+      <c r="BN5">
+        <v>0</v>
+      </c>
+      <c r="BO5">
+        <v>0</v>
+      </c>
+      <c r="BP5">
+        <v>0</v>
+      </c>
+      <c r="BQ5">
+        <v>0</v>
+      </c>
+      <c r="BR5">
+        <v>0</v>
+      </c>
+      <c r="BS5">
+        <v>0</v>
+      </c>
+      <c r="BT5">
+        <v>0</v>
+      </c>
+      <c r="BV5">
+        <v>0</v>
+      </c>
+      <c r="BW5">
+        <v>0</v>
+      </c>
+      <c r="BX5">
+        <v>0</v>
+      </c>
+      <c r="BY5">
+        <v>0</v>
+      </c>
+      <c r="BZ5">
+        <v>0</v>
+      </c>
+      <c r="CA5">
+        <v>0</v>
+      </c>
+      <c r="CB5">
+        <v>0</v>
+      </c>
+      <c r="CC5">
+        <v>0</v>
+      </c>
+      <c r="CD5">
+        <v>0</v>
+      </c>
+      <c r="CE5">
+        <v>0</v>
+      </c>
+      <c r="CF5">
+        <v>0</v>
+      </c>
+      <c r="CG5">
+        <v>0</v>
+      </c>
+      <c r="CT5">
+        <v>0</v>
+      </c>
+      <c r="CU5">
+        <v>0</v>
+      </c>
+      <c r="CV5">
+        <v>0</v>
+      </c>
+      <c r="CW5">
+        <v>0</v>
+      </c>
+      <c r="CX5">
+        <v>0</v>
+      </c>
+      <c r="CY5">
+        <v>1</v>
+      </c>
+      <c r="CZ5">
+        <v>1</v>
+      </c>
+      <c r="DA5">
+        <v>0</v>
+      </c>
+      <c r="DB5">
+        <v>4</v>
+      </c>
+      <c r="DC5">
+        <v>0</v>
+      </c>
+      <c r="DD5">
+        <v>0</v>
+      </c>
+      <c r="DE5">
+        <v>0</v>
+      </c>
+      <c r="DF5">
+        <v>0</v>
+      </c>
+      <c r="DG5">
+        <v>0</v>
+      </c>
+      <c r="DH5">
+        <v>0</v>
+      </c>
+      <c r="DJ5">
+        <v>0</v>
+      </c>
+      <c r="DK5">
+        <v>0</v>
+      </c>
+      <c r="DL5">
+        <v>0</v>
+      </c>
+      <c r="DM5">
+        <v>0</v>
+      </c>
+      <c r="DN5">
+        <v>0</v>
+      </c>
+      <c r="DP5">
+        <v>0</v>
+      </c>
+      <c r="DQ5">
+        <v>0</v>
+      </c>
+      <c r="DR5">
+        <v>0</v>
+      </c>
+      <c r="DS5">
+        <v>0</v>
+      </c>
+      <c r="DT5">
+        <v>0</v>
+      </c>
+      <c r="DU5">
+        <v>0</v>
+      </c>
+      <c r="DV5">
+        <v>0</v>
+      </c>
+      <c r="DW5">
+        <v>4923</v>
+      </c>
+      <c r="DX5" t="s">
+        <v>242</v>
+      </c>
+      <c r="DY5" t="s">
+        <v>242</v>
+      </c>
+      <c r="DZ5">
+        <v>1</v>
+      </c>
+      <c r="EA5">
+        <v>0</v>
+      </c>
+      <c r="EB5">
+        <v>20210401</v>
+      </c>
+      <c r="EC5">
+        <v>99999999</v>
+      </c>
+      <c r="ED5">
+        <v>0</v>
+      </c>
+      <c r="EE5">
+        <v>0</v>
+      </c>
+      <c r="EF5">
+        <v>0</v>
+      </c>
+      <c r="EG5">
+        <v>0</v>
+      </c>
+      <c r="EH5">
+        <v>0</v>
+      </c>
+      <c r="EI5">
+        <v>0</v>
+      </c>
+      <c r="EJ5">
+        <v>0</v>
+      </c>
+      <c r="EK5">
+        <v>0</v>
+      </c>
+      <c r="EL5">
+        <v>0</v>
+      </c>
+      <c r="EM5">
+        <v>0</v>
+      </c>
+      <c r="EN5">
+        <v>0</v>
+      </c>
+      <c r="EO5">
+        <v>0</v>
+      </c>
+      <c r="EP5" t="s">
+        <v>198</v>
+      </c>
+      <c r="EQ5">
+        <v>0</v>
+      </c>
+      <c r="ER5">
+        <v>0</v>
+      </c>
+      <c r="ES5">
+        <v>0</v>
+      </c>
+      <c r="ET5">
+        <v>0</v>
+      </c>
+      <c r="EU5">
+        <v>0</v>
+      </c>
+      <c r="EV5">
+        <v>0</v>
+      </c>
+      <c r="EW5">
+        <v>0</v>
+      </c>
+      <c r="EX5">
+        <v>61040607912</v>
+      </c>
+      <c r="EY5">
+        <v>0</v>
+      </c>
+      <c r="FA5">
+        <v>0</v>
+      </c>
+      <c r="FD5">
+        <v>0</v>
+      </c>
+      <c r="FE5">
+        <v>0</v>
+      </c>
+      <c r="FF5">
+        <v>0</v>
+      </c>
+      <c r="FG5">
+        <v>0</v>
+      </c>
+      <c r="FH5">
+        <v>0</v>
+      </c>
+      <c r="FI5">
+        <v>0</v>
+      </c>
+      <c r="FJ5">
+        <v>0</v>
+      </c>
+      <c r="FK5">
+        <v>0</v>
+      </c>
+      <c r="FL5">
+        <v>0</v>
+      </c>
+      <c r="FM5">
+        <v>0</v>
+      </c>
+      <c r="FN5">
+        <v>0</v>
+      </c>
+      <c r="FO5" t="s">
+        <v>199</v>
+      </c>
+      <c r="FP5">
+        <v>99909</v>
+      </c>
+      <c r="FR5" t="s">
+        <v>199</v>
+      </c>
+      <c r="FS5">
+        <v>99909</v>
+      </c>
+      <c r="FU5">
+        <v>0</v>
+      </c>
+      <c r="FV5">
+        <v>0</v>
+      </c>
+      <c r="FW5">
+        <v>0</v>
+      </c>
+      <c r="FX5">
+        <v>0</v>
+      </c>
+      <c r="FY5">
+        <v>0</v>
+      </c>
+      <c r="FZ5">
+        <v>0</v>
+      </c>
+      <c r="GA5">
+        <v>0</v>
+      </c>
+      <c r="GB5" t="s">
+        <v>196</v>
+      </c>
+      <c r="GC5">
+        <v>0</v>
+      </c>
+      <c r="GD5">
+        <v>0</v>
+      </c>
+      <c r="GE5">
+        <v>0</v>
+      </c>
+      <c r="GF5">
+        <v>0</v>
+      </c>
+      <c r="GG5">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E086942-F573-41A8-ADBE-F11A63D57450}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D1" t="s">
+        <v>248</v>
+      </c>
+      <c r="E1" t="s">
+        <v>249</v>
+      </c>
+      <c r="F1" t="s">
+        <v>250</v>
+      </c>
+      <c r="G1" t="s">
+        <v>223</v>
+      </c>
+      <c r="H1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1" t="s">
+        <v>225</v>
+      </c>
+      <c r="J1" t="s">
+        <v>226</v>
+      </c>
+      <c r="K1" t="s">
+        <v>227</v>
+      </c>
+      <c r="L1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>2008</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>44450.687767337964</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>44450.687767337964</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A7CCF8A-6467-4D9B-AEA6-71DF1E7CD2F8}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3193,7 +3773,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{056702FF-D5C6-47A2-8908-96328535A341}">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -3269,12 +3849,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66585E5F-4455-4306-AEC3-B82B98131596}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3339,7 +3919,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A64569A3-BF18-4653-AA2B-EEF222DCB9A2}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
@@ -3543,7 +4123,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F7B2416-F2DB-4B20-912E-E3AA093AC97B}">
   <dimension ref="A1:L2"/>
   <sheetViews>

</xml_diff>

<commit_message>
add 2 case ut FromHistory
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/TodayOdrRepository/FromHistorySample.xlsx
+++ b/CloudTest/SampleData/TodayOdrRepository/FromHistorySample.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SmartKarteBE\emr-cloud-be\CloudTest\SampleData\TodayOdrRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E9429B-A658-4CB1-8AF0-8F96D2080DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F825AC-C7F5-4703-9FD3-76DE9680D3EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TenMst" sheetId="1" r:id="rId1"/>
-    <sheet name="SystemConf" sheetId="7" state="hidden" r:id="rId2"/>
+    <sheet name="SystemConf" sheetId="7" r:id="rId2"/>
     <sheet name="YohoSetMst" sheetId="4" r:id="rId3"/>
     <sheet name="IpnKasanExclude" sheetId="5" r:id="rId4"/>
     <sheet name="IpnKasanExcludeItem" sheetId="6" r:id="rId5"/>
@@ -3619,8 +3619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E086942-F573-41A8-ADBE-F11A63D57450}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3698,7 +3698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A7CCF8A-6467-4D9B-AEA6-71DF1E7CD2F8}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>